<commit_message>
V0.8.1 Fixes in tests
</commit_message>
<xml_diff>
--- a/builder-eo/src/main/resources/eo.xlsx
+++ b/builder-eo/src/main/resources/eo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/werner.diwischek/dev/elasticobjects/builder-eo/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD14948-7228-4945-B7CF-1B0BDF0485DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB16DF1-9896-E84E-A4BB-378C68614AB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="480" windowWidth="28240" windowHeight="17540" xr2:uid="{1E8B47EF-5738-BE4A-AAD2-1678499A82C4}"/>
+    <workbookView xWindow="1240" yWindow="1120" windowWidth="28240" windowHeight="17540" xr2:uid="{1E8B47EF-5738-BE4A-AAD2-1678499A82C4}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="2" r:id="rId1"/>
@@ -3033,9 +3033,6 @@
     <t>javaGet4Bean</t>
   </si>
   <si>
-    <t>DbSqlConfigInterface, BaseBeanInterface</t>
-  </si>
-  <si>
     <t>{
       "javaDescription": {"default":true, "final": true, "jsonIgnore": true, "transient": true},
       "javaGet4Bean": {"default":true, "final": true, "jsonIgnore": true, "transient": true},
@@ -3057,6 +3054,9 @@
   </si>
   <si>
     <t>expose, module, moduleScope, scope, configModelKey, properties</t>
+  </si>
+  <si>
+    <t>DbSqlConfigInterface,BaseBeanInterface</t>
   </si>
 </sst>
 </file>
@@ -3445,13 +3445,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2949A4-7E1C-7F4B-A1BC-11445B521B01}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
+      <selection pane="bottomRight" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3522,7 +3523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="54" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>146</v>
       </c>
@@ -3551,7 +3552,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>417</v>
       </c>
@@ -3589,7 +3590,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -3615,7 +3616,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="177" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>150</v>
       </c>
@@ -3644,7 +3645,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="153" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>418</v>
       </c>
@@ -3685,7 +3686,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>742</v>
       </c>
@@ -3727,7 +3728,7 @@
         <v>42725</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>873</v>
       </c>
@@ -3769,7 +3770,7 @@
         <v>44186</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>744</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>44186</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>782</v>
       </c>
@@ -3850,7 +3851,7 @@
         <v>44186</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -3882,7 +3883,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="102" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>153</v>
       </c>
@@ -3917,7 +3918,7 @@
         <v>43390</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>534</v>
       </c>
@@ -3953,7 +3954,7 @@
         <v>44144</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="255" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="255" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>156</v>
       </c>
@@ -3995,7 +3996,7 @@
         <v>44023</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>157</v>
       </c>
@@ -4025,7 +4026,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>158</v>
       </c>
@@ -4055,7 +4056,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>239</v>
       </c>
@@ -4094,7 +4095,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>696</v>
       </c>
@@ -4105,7 +4106,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>876</v>
@@ -4136,7 +4137,7 @@
         <v>44181</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>876</v>
       </c>
@@ -4178,7 +4179,7 @@
         <v>44082</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>162</v>
       </c>
@@ -4217,7 +4218,7 @@
         <v>43390</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>743</v>
       </c>
@@ -4259,7 +4260,7 @@
         <v>44181</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>783</v>
       </c>
@@ -4298,7 +4299,7 @@
         <v>44181</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>621</v>
       </c>
@@ -4331,7 +4332,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>165</v>
       </c>
@@ -4370,7 +4371,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>454</v>
       </c>
@@ -4409,7 +4410,7 @@
         <v>44026</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>167</v>
       </c>
@@ -4450,7 +4451,7 @@
         <v>44105</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>614</v>
       </c>
@@ -4486,7 +4487,7 @@
         <v>44081</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>619</v>
       </c>
@@ -4519,7 +4520,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>667</v>
       </c>
@@ -4552,7 +4553,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>171</v>
       </c>
@@ -4590,7 +4591,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>615</v>
       </c>
@@ -4623,7 +4624,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>370</v>
       </c>
@@ -4658,7 +4659,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="102" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>574</v>
       </c>
@@ -4691,7 +4692,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>371</v>
       </c>
@@ -4726,7 +4727,7 @@
         <v>42707</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>520</v>
       </c>
@@ -4768,7 +4769,7 @@
         <v>42707</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>521</v>
       </c>
@@ -4807,7 +4808,7 @@
         <v>42707</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>374</v>
       </c>
@@ -4842,7 +4843,7 @@
         <v>44060</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
@@ -5210,7 +5211,7 @@
         <v>44061</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>812</v>
       </c>
@@ -5224,7 +5225,7 @@
         <v>814</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>35</v>
@@ -5468,7 +5469,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>460</v>
       </c>
@@ -5501,7 +5502,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="119" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>485</v>
       </c>
@@ -5540,7 +5541,7 @@
         <v>44106</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="102" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>498</v>
       </c>
@@ -5579,7 +5580,7 @@
         <v>44114</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="119" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>459</v>
       </c>
@@ -5621,7 +5622,7 @@
         <v>44106</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>632</v>
       </c>
@@ -5660,7 +5661,7 @@
         <v>44128</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>131</v>
       </c>
@@ -5686,7 +5687,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>172</v>
       </c>
@@ -5718,7 +5719,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>174</v>
       </c>
@@ -5747,7 +5748,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>45</v>
       </c>
@@ -5779,7 +5780,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>694</v>
       </c>
@@ -5821,7 +5822,7 @@
         <v>44174</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>767</v>
       </c>
@@ -5860,7 +5861,7 @@
         <v>44181</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="102" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:19" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>746</v>
       </c>
@@ -5902,7 +5903,7 @@
         <v>44145</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="372" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:19" ht="372" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>822</v>
       </c>
@@ -5913,7 +5914,7 @@
         <v>11</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>746</v>
@@ -5938,7 +5939,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>824</v>
       </c>
@@ -5971,7 +5972,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>177</v>
       </c>
@@ -6012,7 +6013,7 @@
         <v>43390</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="102" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:19" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>748</v>
       </c>
@@ -6054,7 +6055,7 @@
         <v>44023</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>752</v>
       </c>
@@ -6099,7 +6100,7 @@
         <v>44144</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>753</v>
       </c>
@@ -6141,7 +6142,7 @@
         <v>44023</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:19" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>606</v>
       </c>
@@ -6177,7 +6178,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>178</v>
       </c>
@@ -6221,7 +6222,7 @@
         <v>44144</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:19" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>787</v>
       </c>
@@ -6260,7 +6261,7 @@
         <v>44083</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>747</v>
       </c>
@@ -6299,7 +6300,7 @@
         <v>44144</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>180</v>
       </c>
@@ -6334,7 +6335,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:19" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>623</v>
       </c>
@@ -6376,7 +6377,7 @@
         <v>44108</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:19" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>181</v>
       </c>
@@ -6417,7 +6418,7 @@
         <v>44108</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>132</v>
       </c>
@@ -6446,7 +6447,7 @@
         <v>44108</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:19" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>712</v>
       </c>
@@ -6485,7 +6486,7 @@
         <v>44105</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>719</v>
       </c>
@@ -6522,7 +6523,7 @@
       </c>
       <c r="P82" s="6"/>
     </row>
-    <row r="83" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>711</v>
       </c>
@@ -6561,7 +6562,7 @@
         <v>44121</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>720</v>
       </c>
@@ -6595,7 +6596,7 @@
       </c>
       <c r="P84" s="6"/>
     </row>
-    <row r="85" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>714</v>
       </c>
@@ -6631,7 +6632,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>717</v>
       </c>
@@ -6664,7 +6665,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>722</v>
       </c>
@@ -6697,7 +6698,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>715</v>
       </c>
@@ -6733,7 +6734,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>455</v>
       </c>
@@ -6772,7 +6773,7 @@
         <v>44108</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>32</v>
       </c>
@@ -6801,7 +6802,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>796</v>
       </c>
@@ -6843,7 +6844,7 @@
         <v>44023</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>909</v>
       </c>
@@ -6882,7 +6883,7 @@
         <v>44181</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>608</v>
       </c>
@@ -6921,7 +6922,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>182</v>
       </c>
@@ -6956,7 +6957,7 @@
         <v>43390</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>790</v>
       </c>
@@ -6995,7 +6996,7 @@
         <v>44093</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>789</v>
       </c>
@@ -7031,7 +7032,7 @@
         <v>44181</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>67</v>
       </c>
@@ -7057,7 +7058,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>120</v>
       </c>
@@ -7083,7 +7084,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>625</v>
       </c>
@@ -7119,7 +7120,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>78</v>
       </c>
@@ -7151,7 +7152,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>188</v>
       </c>
@@ -7183,7 +7184,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>190</v>
       </c>
@@ -7212,7 +7213,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>191</v>
       </c>
@@ -7241,7 +7242,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>192</v>
       </c>
@@ -7270,7 +7271,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" ht="238" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>335</v>
       </c>
@@ -7302,7 +7303,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>83</v>
       </c>
@@ -7334,7 +7335,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>573</v>
       </c>
@@ -7367,7 +7368,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>85</v>
       </c>
@@ -7393,7 +7394,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>39</v>
       </c>
@@ -7419,7 +7420,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>195</v>
       </c>
@@ -7442,7 +7443,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="404" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" ht="404" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>756</v>
       </c>
@@ -7478,7 +7479,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>697</v>
       </c>
@@ -7517,7 +7518,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>768</v>
       </c>
@@ -7556,7 +7557,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>823</v>
       </c>
@@ -7567,7 +7568,7 @@
         <v>11</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>756</v>
@@ -7592,7 +7593,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" ht="238" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>197</v>
       </c>
@@ -7630,7 +7631,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>579</v>
       </c>
@@ -7669,7 +7670,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>580</v>
       </c>
@@ -7705,7 +7706,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="340" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" ht="340" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>482</v>
       </c>
@@ -7741,7 +7742,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>755</v>
       </c>
@@ -7774,7 +7775,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>199</v>
       </c>
@@ -7806,7 +7807,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>201</v>
       </c>
@@ -7838,7 +7839,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>203</v>
       </c>
@@ -7870,7 +7871,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>205</v>
       </c>
@@ -7902,7 +7903,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>207</v>
       </c>
@@ -7934,7 +7935,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>209</v>
       </c>
@@ -7966,7 +7967,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>210</v>
       </c>
@@ -7995,7 +7996,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>133</v>
       </c>
@@ -8024,7 +8025,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>56</v>
       </c>
@@ -8053,7 +8054,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>212</v>
       </c>
@@ -8085,7 +8086,7 @@
         <v>44025</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>214</v>
       </c>
@@ -8117,7 +8118,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>785</v>
       </c>
@@ -8159,7 +8160,7 @@
         <v>44181</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>914</v>
       </c>
@@ -8192,7 +8193,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>786</v>
       </c>
@@ -8231,7 +8232,7 @@
         <v>44181</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>788</v>
       </c>
@@ -8267,7 +8268,7 @@
         <v>44046</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:19" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>794</v>
       </c>
@@ -8303,7 +8304,7 @@
         <v>44046</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>545</v>
       </c>
@@ -8339,7 +8340,7 @@
         <v>44069</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:19" ht="93" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>217</v>
       </c>
@@ -8374,7 +8375,7 @@
         <v>44046</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:19" ht="125" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>220</v>
       </c>
@@ -8406,7 +8407,7 @@
         <v>44046</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>125</v>
       </c>
@@ -8441,7 +8442,7 @@
         <v>44046</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>222</v>
       </c>
@@ -8473,7 +8474,7 @@
         <v>44046</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>636</v>
       </c>
@@ -8509,7 +8510,7 @@
         <v>44046</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>223</v>
       </c>
@@ -8548,7 +8549,7 @@
         <v>43390</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>664</v>
       </c>
@@ -8584,7 +8585,7 @@
         <v>44123</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>13</v>
       </c>
@@ -8613,7 +8614,7 @@
         <v>44041</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>225</v>
       </c>
@@ -8646,7 +8647,7 @@
         <v>44100</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>226</v>
       </c>
@@ -8679,7 +8680,7 @@
         <v>44070</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>227</v>
       </c>
@@ -8715,7 +8716,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="118" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:19" ht="118" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>737</v>
       </c>
@@ -8754,7 +8755,7 @@
         <v>44046</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>736</v>
       </c>
@@ -8790,7 +8791,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>229</v>
       </c>
@@ -8829,7 +8830,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>409</v>
       </c>
@@ -8868,7 +8869,7 @@
         <v>44060</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>415</v>
       </c>
@@ -8905,7 +8906,7 @@
       </c>
       <c r="S152" s="7"/>
     </row>
-    <row r="153" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>231</v>
       </c>
@@ -8942,7 +8943,7 @@
       </c>
       <c r="S153" s="7"/>
     </row>
-    <row r="154" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>233</v>
       </c>
@@ -8979,7 +8980,7 @@
       </c>
       <c r="S154" s="7"/>
     </row>
-    <row r="155" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>234</v>
       </c>
@@ -9019,7 +9020,7 @@
       </c>
       <c r="S155" s="7"/>
     </row>
-    <row r="156" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:19" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>528</v>
       </c>
@@ -9055,7 +9056,7 @@
         <v>44141</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>236</v>
       </c>
@@ -9091,7 +9092,7 @@
         <v>44141</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>399</v>
       </c>
@@ -9125,7 +9126,7 @@
       </c>
       <c r="S158" s="7"/>
     </row>
-    <row r="159" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>250</v>
       </c>
@@ -9167,7 +9168,7 @@
         <v>44141</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>583</v>
       </c>
@@ -9200,7 +9201,7 @@
         <v>44141</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>237</v>
       </c>
@@ -9241,7 +9242,7 @@
         <v>44141</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:19" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>253</v>
       </c>
@@ -9276,7 +9277,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:19" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>819</v>
       </c>
@@ -9312,7 +9313,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:19" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>256</v>
       </c>
@@ -9352,6 +9353,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N164" xr:uid="{A955F0F7-5ED5-4A4E-94AE-7EA930688524}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="eo-db"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:N151">
       <sortCondition ref="A2:A151"/>
     </sortState>

</xml_diff>